<commit_message>
Updates on natives interaction
Beggining of the development of some native interactions such as gift native units and recruit them
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint 1/Burndown chart.xlsx
+++ b/Project_Management/Sprint 1/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubRepos\ES\SE2324_62475_61891\Project_Management\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8BD54E7-2F60-45BC-B26E-1FCF4621CFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5EEF0-2C36-4F78-B1BA-B919EFD4E794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16725" yWindow="6165" windowWidth="14745" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -565,6 +565,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,9 +615,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2155,7 +2155,7 @@
   <dimension ref="B1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,72 +2163,72 @@
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="40"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="42"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="43"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="4">
+        <v>45259</v>
+      </c>
+      <c r="F4" s="4">
         <v>45260</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>45261</v>
-      </c>
-      <c r="G4" s="4">
-        <v>45262</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -2236,8 +2236,8 @@
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="32"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="B9" s="22">
         <v>4</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="25">
@@ -2410,15 +2410,15 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="2">
         <v>0</v>
       </c>
       <c r="E16" s="14">
-        <f t="shared" ref="E16:K16" si="0">SUM(E6:E15)</f>
+        <f t="shared" ref="E16:G16" si="0">SUM(E6:E15)</f>
         <v>6</v>
       </c>
       <c r="F16" s="14">
@@ -2435,16 +2435,16 @@
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="16">
         <f>SUM(D6:D16)</f>
         <v>11</v>
       </c>
       <c r="E17" s="17">
-        <f t="shared" ref="E17:K17" si="1">D17-SUM(E6:E15)</f>
+        <f t="shared" ref="E17:G17" si="1">D17-SUM(E6:E15)</f>
         <v>5</v>
       </c>
       <c r="F17" s="15">
@@ -2461,10 +2461,10 @@
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="28">
         <f>D17</f>
         <v>11</v>

</xml_diff>